<commit_message>
10-May-2015  Reconcile Page (Amount will be modified by now)
</commit_message>
<xml_diff>
--- a/src/test/java/config/DataTable.xlsx
+++ b/src/test/java/config/DataTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin.kumar\git\MyVision\src\test\java\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin.kumar\git\TFE\src\test\java\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12435" windowWidth="25125" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" windowHeight="12435" windowWidth="25125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="loginQA" r:id="rId1" sheetId="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="46">
   <si>
     <t>UserName</t>
   </si>
@@ -147,46 +147,25 @@
     <t>DEV4</t>
   </si>
   <si>
-    <t>00997507</t>
-  </si>
-  <si>
-    <t>00997507 - 2017 Chevrolet Express 2500 Work Van Rear-wheel Drive Cargo Van (CG23405)</t>
+    <t>00997989</t>
+  </si>
+  <si>
+    <t>00997989 - 2017 Ford F-450 Chassis XL 4x2 SD Crew Cab 179 in. WB DRW (W4G)</t>
   </si>
   <si>
     <t>AAAAAAAAAAAAAAAAA</t>
   </si>
   <si>
-    <t>00158470 - Al Piemonte Chevrolet</t>
-  </si>
-  <si>
-    <t>$200.00</t>
-  </si>
-  <si>
-    <t>PON00211768/0</t>
-  </si>
-  <si>
-    <t>INV00211768</t>
-  </si>
-  <si>
-    <t>$27,914.50</t>
-  </si>
-  <si>
-    <t>PON00211766/0</t>
-  </si>
-  <si>
-    <t>INV00211766</t>
-  </si>
-  <si>
-    <t>00087859 - Carl's Stereo Plus Pickups</t>
-  </si>
-  <si>
-    <t>$1,985.17</t>
-  </si>
-  <si>
-    <t>PON00211767/0</t>
-  </si>
-  <si>
-    <t>INV00211767</t>
+    <t>00044002 - Al Piemonte Ford Sales Inc</t>
+  </si>
+  <si>
+    <t>$33,044.00</t>
+  </si>
+  <si>
+    <t>PON00212643/0</t>
+  </si>
+  <si>
+    <t>INV00212643</t>
   </si>
 </sst>
 </file>
@@ -573,7 +552,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -868,14 +847,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="82.34375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.67578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.71875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.84375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.98046875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.2578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.6171875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.93359375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="5.05078125" collapsed="false"/>
+    <col min="7" max="7" width="12.43359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -926,61 +904,6 @@
       <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
10-May-2017 MainPO, Reclaims, CD Fee will be modified by now
</commit_message>
<xml_diff>
--- a/src/test/java/config/DataTable.xlsx
+++ b/src/test/java/config/DataTable.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin.kumar\git\TFE\src\test\java\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="12435" windowWidth="25125" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="loginQA" r:id="rId1" sheetId="1"/>
-    <sheet name="Unit to Reconcile" r:id="rId2" sheetId="4"/>
-    <sheet name="PO_Detail" r:id="rId3" sheetId="2"/>
-    <sheet name="acceptQueue" r:id="rId4" sheetId="3"/>
-    <sheet name="Unit_to_Reconcile_Output" r:id="rId9" sheetId="5"/>
+    <sheet name="loginQA" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit to Reconcile" sheetId="4" r:id="rId2"/>
+    <sheet name="PO_Detail" sheetId="2" r:id="rId3"/>
+    <sheet name="acceptQueue" sheetId="3" r:id="rId4"/>
+    <sheet name="Unit_to_Reconcile_Output" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>UserName</t>
   </si>
@@ -126,9 +126,6 @@
     <t>DEV2</t>
   </si>
   <si>
-    <t>336985</t>
-  </si>
-  <si>
     <t>QA3</t>
   </si>
   <si>
@@ -147,32 +144,16 @@
     <t>DEV4</t>
   </si>
   <si>
-    <t>00997989</t>
-  </si>
-  <si>
-    <t>00997989 - 2017 Ford F-450 Chassis XL 4x2 SD Crew Cab 179 in. WB DRW (W4G)</t>
-  </si>
-  <si>
-    <t>AAAAAAAAAAAAAAAAA</t>
-  </si>
-  <si>
-    <t>00044002 - Al Piemonte Ford Sales Inc</t>
-  </si>
-  <si>
-    <t>$33,044.00</t>
-  </si>
-  <si>
-    <t>PON00212643/0</t>
-  </si>
-  <si>
-    <t>INV00212643</t>
+    <t>366965</t>
+  </si>
+  <si>
+    <t>00998376</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -244,37 +225,37 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -291,10 +272,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -329,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,7 +345,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,21 +439,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -489,7 +470,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -541,14 +522,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -557,13 +538,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -637,13 +618,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -654,13 +635,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -705,7 +686,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>13</v>
@@ -722,13 +703,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -750,15 +731,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -767,7 +748,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -776,26 +757,24 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -804,22 +783,22 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,32 +810,23 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.84375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.98046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.2578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.6171875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="5.05078125" collapsed="false"/>
-    <col min="7" max="7" width="12.43359375" customWidth="true" bestFit="true"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -882,30 +852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
10-May-2017   PO018(Vehicle Order Status) Script added
</commit_message>
<xml_diff>
--- a/src/test/java/config/DataTable.xlsx
+++ b/src/test/java/config/DataTable.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>UserName</t>
   </si>
@@ -144,10 +144,52 @@
     <t>DEV4</t>
   </si>
   <si>
-    <t>366965</t>
-  </si>
-  <si>
-    <t>00998376</t>
+    <t>366231</t>
+  </si>
+  <si>
+    <t>00998377</t>
+  </si>
+  <si>
+    <t>00998377 - 2017 Toyota Corolla LE 4dr Sedan (1852)</t>
+  </si>
+  <si>
+    <t>AAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>00057063 - Scott Clarks Toyota City</t>
+  </si>
+  <si>
+    <t>$16,534.95</t>
+  </si>
+  <si>
+    <t>PON00213541/0</t>
+  </si>
+  <si>
+    <t>INV00213541</t>
+  </si>
+  <si>
+    <t>$17,903.00</t>
+  </si>
+  <si>
+    <t>$300.00</t>
+  </si>
+  <si>
+    <t>PON00213542/0</t>
+  </si>
+  <si>
+    <t>INV00213542</t>
+  </si>
+  <si>
+    <t>$375.00</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>DA?</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -766,10 +808,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,13 +819,25 @@
     <col min="1" max="1" width="17.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -798,7 +852,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,11 +874,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -852,6 +916,58 @@
         <v>30</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UNTREC now get the QUOTED AMOUNT instead of INVOICING AMOUNT
</commit_message>
<xml_diff>
--- a/src/test/java/config/DataTable.xlsx
+++ b/src/test/java/config/DataTable.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="loginQA" sheetId="1" r:id="rId1"/>
     <sheet name="PO_Detail" sheetId="2" r:id="rId2"/>
-    <sheet name="Unit_to_Reconcile_Output" sheetId="5" r:id="rId3"/>
+    <sheet name="Unit_to_Reconcile_Output" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>UserName</t>
   </si>
@@ -136,61 +136,52 @@
     <t>DEV4</t>
   </si>
   <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>DA?</t>
+  </si>
+  <si>
+    <t>In Service Date</t>
+  </si>
+  <si>
+    <t>05/01/2017</t>
+  </si>
+  <si>
+    <t>grover</t>
+  </si>
+  <si>
+    <t>Mal@0000</t>
+  </si>
+  <si>
+    <t>369185</t>
+  </si>
+  <si>
+    <t>00998503</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>00998503 - 2017 Chevrolet Express 2500 Work Van Rear-wheel Drive Cargo Van (CG23405)</t>
+  </si>
+  <si>
     <t>AAAAAAAAAAAAAAAAA</t>
   </si>
   <si>
-    <t>00057063 - Scott Clarks Toyota City</t>
-  </si>
-  <si>
-    <t>$16,534.95</t>
-  </si>
-  <si>
-    <t>$17,903.00</t>
-  </si>
-  <si>
-    <t>$300.00</t>
-  </si>
-  <si>
-    <t>$375.00</t>
-  </si>
-  <si>
-    <t>Quote</t>
-  </si>
-  <si>
-    <t>DA?</t>
-  </si>
-  <si>
-    <t>366207</t>
-  </si>
-  <si>
-    <t>00998382</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>00998382 - 2017 Toyota Corolla LE 4dr Sedan (1852)</t>
-  </si>
-  <si>
-    <t>PON00213549/0</t>
-  </si>
-  <si>
-    <t>INV00213549</t>
-  </si>
-  <si>
-    <t>PON00213550/0</t>
-  </si>
-  <si>
-    <t>INV00213550</t>
-  </si>
-  <si>
-    <t>00967052</t>
-  </si>
-  <si>
-    <t>In Service Date</t>
-  </si>
-  <si>
-    <t>04/01/2017</t>
+    <t>00158470 - Al Piemonte Chevrolet</t>
+  </si>
+  <si>
+    <t>$24,914.50</t>
+  </si>
+  <si>
+    <t>PON00213850/0</t>
+  </si>
+  <si>
+    <t>INV00213850</t>
+  </si>
+  <si>
+    <t>00995845</t>
   </si>
 </sst>
 </file>
@@ -576,7 +567,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +628,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -775,9 +772,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -786,7 +784,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,30 +796,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -832,22 +830,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -878,54 +873,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
         <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Matrix Rain Effect added to the report module
</commit_message>
<xml_diff>
--- a/src/test/java/config/DataTable.xlsx
+++ b/src/test/java/config/DataTable.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin.kumar\git\TFE\src\test\java\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435" activeTab="2"/>
+    <workbookView activeTab="1" windowHeight="12435" windowWidth="25125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="loginQA" sheetId="1" r:id="rId1"/>
-    <sheet name="PO_Detail" sheetId="2" r:id="rId2"/>
-    <sheet name="Unit_to_Reconcile_Output" sheetId="5" r:id="rId3"/>
+    <sheet name="loginQA" r:id="rId1" sheetId="1"/>
+    <sheet name="PO_Detail" r:id="rId2" sheetId="2"/>
+    <sheet name="Unit_to_Reconcile_Output" r:id="rId3" sheetId="5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>UserName</t>
   </si>
@@ -151,22 +151,20 @@
     <t>Mal@0000</t>
   </si>
   <si>
-    <t>07/01/2017</t>
-  </si>
-  <si>
-    <t>382245</t>
-  </si>
-  <si>
-    <t>00999159</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>382425</t>
+  </si>
+  <si>
+    <t>00999166</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,38 +236,38 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -286,10 +284,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -324,7 +322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,7 +357,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,21 +451,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -484,7 +482,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -536,14 +534,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -552,13 +550,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -751,27 +749,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="17.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="4.6796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,29 +788,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="D2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -845,6 +841,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last Day at R Systems
</commit_message>
<xml_diff>
--- a/src/test/java/config/DataTable.xlsx
+++ b/src/test/java/config/DataTable.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin.kumar\git\TFE\src\test\java\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12435" windowWidth="25125" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="loginQA" r:id="rId1" sheetId="1"/>
-    <sheet name="PO_Detail" r:id="rId2" sheetId="2"/>
-    <sheet name="Unit_to_Reconcile_Output" r:id="rId3" sheetId="5"/>
+    <sheet name="loginQA" sheetId="1" r:id="rId1"/>
+    <sheet name="PO_Detail" sheetId="2" r:id="rId2"/>
+    <sheet name="Unit_to_Reconcile_Output" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>UserName</t>
   </si>
@@ -151,20 +151,34 @@
     <t>Mal@0000</t>
   </si>
   <si>
-    <t>382425</t>
-  </si>
-  <si>
-    <t>00999166</t>
+    <t>01000996</t>
+  </si>
+  <si>
+    <t>01000949</t>
+  </si>
+  <si>
+    <t>01000942</t>
+  </si>
+  <si>
+    <t>01000943</t>
+  </si>
+  <si>
+    <t>01001011</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Stuck on UNTPRG-Confirm PO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,38 +250,38 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -284,10 +298,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -322,7 +336,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,7 +371,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,21 +465,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -482,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -534,14 +548,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -550,13 +564,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -749,27 +763,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="17.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="4.6796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.703125" collapsed="true"/>
+    <col min="1" max="1" width="17.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,25 +801,60 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -841,6 +890,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>